<commit_message>
Output data first tests
Please find here an update for our output data. I moved Francis's spreadsheet into the output file and added data from our first active learning.
In the data folder, I added a labware glossary.
</commit_message>
<xml_diff>
--- a/data/2023.10.25-JS.xlsx
+++ b/data/2023.10.25-JS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinkp\GitHub\opentrons\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b59e0684c1115e5a/Documents/GitHub/opentrons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF9B86-35C8-493F-929D-D939DD9085A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_9C6233A21ED810CC451A68B59751A46FA17056CF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{313B061C-6726-4951-A17E-C871ED45E42D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dispense_Volumes" sheetId="1" r:id="rId1"/>
@@ -406,47 +406,47 @@
     <t>Type</t>
   </si>
   <si>
-    <t>nest_96_wellplate_200ul_flat</t>
-  </si>
-  <si>
-    <t>NEST 96 Well Plate 100 µL PCR Full Skirt</t>
-  </si>
-  <si>
     <t>Destination_Wells</t>
   </si>
   <si>
     <t>Stock_Solutions</t>
   </si>
   <si>
-    <t>opentrons_96_tiprack_300ul</t>
-  </si>
-  <si>
-    <t>Opentrons 96 Tip Rack 300 µL</t>
-  </si>
-  <si>
     <t>Tips_Rack</t>
   </si>
   <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>p300_single_gen2</t>
-  </si>
-  <si>
-    <t>Pipette 300uL</t>
-  </si>
-  <si>
-    <t>opentrons_24_tuberack_eppendorf_2ml_safelock_snapcap</t>
-  </si>
-  <si>
-    <t>Opentrons 24 Tube Rack with Eppendorf 2 mL Safe-Lock Snapcap</t>
+    <t>left</t>
+  </si>
+  <si>
+    <t>p20_single_gen2</t>
+  </si>
+  <si>
+    <t>Pipette 20uL</t>
+  </si>
+  <si>
+    <t>corning_24_wellplate_3.4ml_flat</t>
+  </si>
+  <si>
+    <t>corning_96_wellplate_360ul_flat</t>
+  </si>
+  <si>
+    <t>opentrons_96_tiprack_20ul</t>
+  </si>
+  <si>
+    <t>Opentrons 96 Tip Rack 20 µL</t>
+  </si>
+  <si>
+    <t>Corning 96 Well Plate 360 µL Flat</t>
+  </si>
+  <si>
+    <t>Corning 24 Well Plate 3.4 mL Flat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -459,6 +459,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -481,9 +487,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,9 +812,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -934,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -999,7 +1009,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1064,7 +1074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1129,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1194,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1259,7 +1269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1324,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1454,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1519,7 +1529,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1584,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1649,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1714,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1779,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1844,7 +1854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1909,7 +1919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1974,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1</v>
       </c>
@@ -2039,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2104,7 +2114,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2169,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2234,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2364,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2429,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2494,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2559,7 +2569,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2624,7 +2634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2689,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2754,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2819,7 +2829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2884,7 +2894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2949,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -3014,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>1</v>
       </c>
@@ -3079,7 +3089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3144,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>1</v>
       </c>
@@ -3209,7 +3219,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3274,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3339,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1</v>
       </c>
@@ -3404,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3469,7 +3479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3534,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>1</v>
       </c>
@@ -3599,7 +3609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3664,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>1</v>
       </c>
@@ -3729,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3794,7 +3804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>1</v>
       </c>
@@ -3859,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3924,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3989,7 +3999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>1</v>
       </c>
@@ -4054,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1</v>
       </c>
@@ -4119,7 +4129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
@@ -4184,7 +4194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>1</v>
       </c>
@@ -4249,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4314,7 +4324,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
@@ -4379,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1</v>
       </c>
@@ -4444,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
@@ -4509,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1</v>
       </c>
@@ -4574,7 +4584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -4639,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1</v>
       </c>
@@ -4704,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1</v>
       </c>
@@ -4769,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>1</v>
       </c>
@@ -4834,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
@@ -4899,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1</v>
       </c>
@@ -4964,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1</v>
       </c>
@@ -5029,7 +5039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1</v>
       </c>
@@ -5094,7 +5104,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1</v>
       </c>
@@ -5159,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>1</v>
       </c>
@@ -5224,7 +5234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
@@ -5289,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1</v>
       </c>
@@ -5354,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>1</v>
       </c>
@@ -5419,7 +5429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
@@ -5484,7 +5494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>1</v>
       </c>
@@ -5549,7 +5559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1</v>
       </c>
@@ -5614,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -5679,7 +5689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>1</v>
       </c>
@@ -5744,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1</v>
       </c>
@@ -5809,7 +5819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1</v>
       </c>
@@ -5874,7 +5884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>1</v>
       </c>
@@ -5939,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1</v>
       </c>
@@ -6004,7 +6014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>1</v>
       </c>
@@ -6069,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1</v>
       </c>
@@ -6134,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1</v>
       </c>
@@ -6199,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1</v>
       </c>
@@ -6264,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>1</v>
       </c>
@@ -6329,7 +6339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>1</v>
       </c>
@@ -6394,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>1</v>
       </c>
@@ -6459,7 +6469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>1</v>
       </c>
@@ -6524,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1</v>
       </c>
@@ -6589,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1</v>
       </c>
@@ -6654,7 +6664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1</v>
       </c>
@@ -6719,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1</v>
       </c>
@@ -6784,7 +6794,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1</v>
       </c>
@@ -6849,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1</v>
       </c>
@@ -6914,7 +6924,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1</v>
       </c>
@@ -6979,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1</v>
       </c>
@@ -7044,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>1</v>
       </c>
@@ -7109,7 +7119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2</v>
       </c>
@@ -7174,7 +7184,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2</v>
       </c>
@@ -7239,7 +7249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2</v>
       </c>
@@ -7304,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2</v>
       </c>
@@ -7369,7 +7379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2</v>
       </c>
@@ -7434,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2</v>
       </c>
@@ -7499,7 +7509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2</v>
       </c>
@@ -7564,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2</v>
       </c>
@@ -7629,7 +7639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2</v>
       </c>
@@ -7694,7 +7704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2</v>
       </c>
@@ -7759,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>2</v>
       </c>
@@ -7824,7 +7834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>2</v>
       </c>
@@ -7889,7 +7899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2</v>
       </c>
@@ -7954,7 +7964,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2</v>
       </c>
@@ -8019,7 +8029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2</v>
       </c>
@@ -8084,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2</v>
       </c>
@@ -8149,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2</v>
       </c>
@@ -8214,7 +8224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2</v>
       </c>
@@ -8279,7 +8289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2</v>
       </c>
@@ -8344,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2</v>
       </c>
@@ -8409,7 +8419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2</v>
       </c>
@@ -8474,7 +8484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2</v>
       </c>
@@ -8539,7 +8549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2</v>
       </c>
@@ -8604,7 +8614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2</v>
       </c>
@@ -8669,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2</v>
       </c>
@@ -8734,7 +8744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2</v>
       </c>
@@ -8799,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2</v>
       </c>
@@ -8864,7 +8874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2</v>
       </c>
@@ -8929,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2</v>
       </c>
@@ -8994,7 +9004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2</v>
       </c>
@@ -9059,7 +9069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2</v>
       </c>
@@ -9124,7 +9134,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2</v>
       </c>
@@ -9189,7 +9199,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2</v>
       </c>
@@ -9254,7 +9264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2</v>
       </c>
@@ -9319,7 +9329,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2</v>
       </c>
@@ -9384,7 +9394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>2</v>
       </c>
@@ -9449,7 +9459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>2</v>
       </c>
@@ -9514,7 +9524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>2</v>
       </c>
@@ -9579,7 +9589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2</v>
       </c>
@@ -9644,7 +9654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2</v>
       </c>
@@ -9709,7 +9719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2</v>
       </c>
@@ -9774,7 +9784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2</v>
       </c>
@@ -9839,7 +9849,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2</v>
       </c>
@@ -9904,7 +9914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2</v>
       </c>
@@ -9969,7 +9979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2</v>
       </c>
@@ -10034,7 +10044,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2</v>
       </c>
@@ -10099,7 +10109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2</v>
       </c>
@@ -10164,7 +10174,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>2</v>
       </c>
@@ -10229,7 +10239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2</v>
       </c>
@@ -10294,7 +10304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2</v>
       </c>
@@ -10359,7 +10369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2</v>
       </c>
@@ -10424,7 +10434,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>2</v>
       </c>
@@ -10489,7 +10499,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>2</v>
       </c>
@@ -10554,7 +10564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2</v>
       </c>
@@ -10619,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>2</v>
       </c>
@@ -10684,7 +10694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>2</v>
       </c>
@@ -10749,7 +10759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>2</v>
       </c>
@@ -10814,7 +10824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>2</v>
       </c>
@@ -10879,7 +10889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>2</v>
       </c>
@@ -10944,7 +10954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>2</v>
       </c>
@@ -11009,7 +11019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>2</v>
       </c>
@@ -11074,7 +11084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2</v>
       </c>
@@ -11139,7 +11149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2</v>
       </c>
@@ -11204,7 +11214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2</v>
       </c>
@@ -11269,7 +11279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>2</v>
       </c>
@@ -11334,7 +11344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>2</v>
       </c>
@@ -11399,7 +11409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>2</v>
       </c>
@@ -11464,7 +11474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>2</v>
       </c>
@@ -11529,7 +11539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>2</v>
       </c>
@@ -11594,7 +11604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>2</v>
       </c>
@@ -11659,7 +11669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>2</v>
       </c>
@@ -11724,7 +11734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>2</v>
       </c>
@@ -11789,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>2</v>
       </c>
@@ -11854,7 +11864,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>2</v>
       </c>
@@ -11919,7 +11929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>2</v>
       </c>
@@ -11984,7 +11994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>2</v>
       </c>
@@ -12049,7 +12059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>2</v>
       </c>
@@ -12114,7 +12124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>2</v>
       </c>
@@ -12179,7 +12189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>2</v>
       </c>
@@ -12244,7 +12254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2</v>
       </c>
@@ -12309,7 +12319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>2</v>
       </c>
@@ -12374,7 +12384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>2</v>
       </c>
@@ -12439,7 +12449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>2</v>
       </c>
@@ -12504,7 +12514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2</v>
       </c>
@@ -12569,7 +12579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>2</v>
       </c>
@@ -12634,7 +12644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>2</v>
       </c>
@@ -12699,7 +12709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>2</v>
       </c>
@@ -12764,7 +12774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>2</v>
       </c>
@@ -12829,7 +12839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>2</v>
       </c>
@@ -12894,7 +12904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>2</v>
       </c>
@@ -12959,7 +12969,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>2</v>
       </c>
@@ -13024,7 +13034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2</v>
       </c>
@@ -13089,7 +13099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>2</v>
       </c>
@@ -13154,7 +13164,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>2</v>
       </c>
@@ -13219,7 +13229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2</v>
       </c>
@@ -13284,7 +13294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2</v>
       </c>
@@ -13362,14 +13372,14 @@
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>117</v>
       </c>
@@ -13383,7 +13393,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -13397,7 +13407,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -13411,7 +13421,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -13425,7 +13435,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -13439,7 +13449,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -13453,7 +13463,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -13467,7 +13477,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -13481,7 +13491,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -13495,7 +13505,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -13509,7 +13519,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -13523,7 +13533,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -13537,7 +13547,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -13551,7 +13561,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -13565,7 +13575,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -13579,7 +13589,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -13593,7 +13603,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -13607,7 +13617,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -13621,7 +13631,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -13635,7 +13645,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -13658,13 +13668,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="50.81640625" customWidth="1"/>
+    <col min="3" max="3" width="55.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13678,60 +13693,60 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" t="s">
         <v>127</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
         <v>128</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -13743,11 +13758,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="21.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -13758,15 +13778,15 @@
         <v>126</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>